<commit_message>
Updating Title Cells in Data1.csv
</commit_message>
<xml_diff>
--- a/data1.xlsx
+++ b/data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d2f7e3ad783ba04/Desktop/Study_Material/SURA/workspace/Library_Inventory_Management_System/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{DA05008D-D12F-427A-A010-714148B95798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B5AC319-3F25-4D86-9A06-AE867242EEAC}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{DA05008D-D12F-427A-A010-714148B95798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF5DB0C9-FD1F-497B-9DE2-164AFBCCBCD0}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="216" windowWidth="22812" windowHeight="12144" xr2:uid="{01B6461D-C73B-47DD-B185-D00092A47D4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Title</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Materials Science in Construction</t>
+  </si>
+  <si>
+    <t>Checked</t>
   </si>
 </sst>
 </file>
@@ -415,77 +418,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FA82FD-726D-4A27-B7E4-53BC215D76B8}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="68.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>